<commit_message>
Added Enterprise Architect artefacts
</commit_message>
<xml_diff>
--- a/Requirements/Functional Requirements.xlsx
+++ b/Requirements/Functional Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caeta\Desktop\Documents\Proyectos\TimeAdministrator\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caeta\Desktop\Documents\Proyectos\TimeAdministrator\TimeAdministrator\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125B334-3421-4923-B666-CA1C75DE3126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA6D418-B9E2-4931-A958-2EEE3DA2D87F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20910" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Specification date</t>
   </si>
@@ -60,12 +60,6 @@
     <t>System has to allow that de user can create a workspace in which its store his personal configuration for that each time  that user enter to the program its load automatically that workspace</t>
   </si>
   <si>
-    <t>Dark Theme</t>
-  </si>
-  <si>
-    <t>The theme of the program has to be dark. Predominant dark grey</t>
-  </si>
-  <si>
     <t>Load last workspace</t>
   </si>
   <si>
@@ -90,10 +84,10 @@
     <t>The option "Delete Time Register" of the context menu unfolded from the table it has to allow delete from the database the time register of the row in which it was right clicked</t>
   </si>
   <si>
-    <t>Activities labels</t>
-  </si>
-  <si>
     <t>The system it has to detect new labels when an register it's entered or use previous registered labels</t>
+  </si>
+  <si>
+    <t>Manage activities labels</t>
   </si>
 </sst>
 </file>
@@ -109,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +113,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE0D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBAE18F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -172,6 +172,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -182,6 +191,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBAE18F"/>
       <color rgb="FFFFE0D9"/>
       <color rgb="FFFF967D"/>
       <color rgb="FFFF6D4B"/>
@@ -461,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,17 +529,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="9">
         <v>44183</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44183</v>
       </c>
@@ -540,11 +550,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>44183</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>44186</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -556,10 +566,10 @@
         <v>44186</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -567,33 +577,27 @@
         <v>44186</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44186</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>44186</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -621,9 +625,9 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -680,11 +684,6 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>